<commit_message>
Writing output to file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,447 +19,438 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
-  <si>
-    <t>SE-MT-007.000 Temp Census</t>
-  </si>
-  <si>
-    <t>SE-MT-008.000 Med Supp - Quoting</t>
-  </si>
-  <si>
-    <t>SE-NFR-004.005 Inactivity Action</t>
-  </si>
-  <si>
-    <t>SE-PM-007.001 Open Enrollment Ends</t>
-  </si>
-  <si>
-    <t>SE-065-008.001 Supress RSC Lite Access Points</t>
-  </si>
-  <si>
-    <t>SE-IFA-001.000 Saved Individual and Family Applications</t>
-  </si>
-  <si>
-    <t>SE-O65-008.001.001 Supress RSC Lite Access Points:Choose a Different Plan</t>
-  </si>
-  <si>
-    <t>SE-EI-001.004.003.001.003 Census: Temp Only Contingency Functionality</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004.001- Producer Quote - Dental :Valid</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004.001.001 - Producer Quote - Dental: U21</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004.001.002 - Producer Quote - Dental: Mixed</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004.001.003 - Producer Quote - Dental: 21 and Over</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004.001.004 - Producer Quote - Dental: Validation</t>
-  </si>
-  <si>
-    <t>SE-EI-013.006 Login and Elgibility Fetch</t>
-  </si>
-  <si>
-    <t>SE-EI-013.001B.001 Logged In on Public Site</t>
-  </si>
-  <si>
-    <t>SE-EI-005.016.006.004.001.002.002 Warning Page - On Exchange Plan w Estimate Call to Action</t>
-  </si>
-  <si>
-    <t>SE-EI-005.017.002 Plan Results Catastrophic Plans are not Tax Credit Eligible</t>
-  </si>
-  <si>
-    <t>SE-EI-005.018.002 - Plan Details: OOC Link</t>
-  </si>
-  <si>
-    <t>SE-EI-008.025 Confirm and Enroll: Prevent MAJOR MED Enrollment</t>
-  </si>
-  <si>
-    <t>SE-EI-008.024.002 Confirm and Enroll C: Coinsurance -1</t>
-  </si>
-  <si>
-    <t>SE-EI-008.025 Confirm and Enroll: Prevent MARJO MED Enrollment - No Release</t>
-  </si>
-  <si>
-    <t>SE-EI-008.025 Confirm and Enroll: Prevent MAJOR MED Enrollment - No Release</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.012.017.001 Eligibility Response: Applicant Eligibility - CSR Levels Across an Enrollment Group</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.007 Eligibility Response: Enrollment Period - SEP Eligibility Indicator</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.008 Eligibility Response: Enrollment Period - SEP Eligibility Reason</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.009 Eligibility Response: Enrollment Period - SEP Start Date</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.010 Eligibility Response: Enrollment Period - SEP End Date</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.011 Eligibility Response: Enrollment Period - SEP Earliest QHP Effective Date</t>
-  </si>
-  <si>
-    <t>SE-EI-011.001.013.012 Eligibility Response: Enrollment Period - SEP Latest QHP Effective Date</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.001 Return from Exchange: Application Incomplete upon Login</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.002 Return from Exchange: Application Incomplete upon Login Secondary Call to Action</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.003 Return from Exchange: Application Incomplete - Do not display an Applicant Data</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.004 Return from Exchange: Application Incomplete - Transfer Types</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.001.001 Return from Exchange: Application Incomplete upon Login - My Account</t>
-  </si>
-  <si>
-    <t>SE-EI-013.003.002.002.001 Return from Exchange: Application Incomplete upon Login - Go Back to the Exchange</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.062 Enrollment: Payment - List Bill</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064 Enrollment: Payment - List Bill</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.065 Enrollment: Payment - List Bill</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.066 Enrollment: Payment - List Bill</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.059.001 Enrollment: Payment - Billing Address Verification</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.059.001.001 Enrollment: Payment - Billing Address Verification Errors</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.062.001 Enrollment: Payment - List Bill States</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.062.002 Enrollment: Payment - List Bill OX</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.001 Enrollment: Payment - List Bill Number Max Characters</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.002 Enrollment: Payment - List Bill Valid Number</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.003 Enrollment: Payment - List Bill Error Message</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.004 Enrollment: Payment - List Bill Name</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.005 Enrollment: Payment - List Bill Billing Address</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.006 Enrollment: Payment - List Bill Contact Phone Number</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.063 Enrollment: Payment - List Bill Note</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.001.001 Enrollment: Payment - List Bill Number Max Characters</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.004.001 Enrollment: Payment - List Bill Name</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.005.001 Enrollment: Payment - List Bill Billing Address</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.005.002 Enrollment: Payment - List Bill Billing Address</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.005.003 Enrollment: Payment - List Bill Billing Address</t>
-  </si>
-  <si>
-    <t>SE-EI-017.001.064.005.004 Enrollment: Payment - List Bill Billing Address</t>
-  </si>
-  <si>
-    <t>SE-EI-001.018.004 - Producer Quote - Dental</t>
-  </si>
-  <si>
-    <t>SE-WE-001.004 IPA Invalid Product</t>
-  </si>
-  <si>
-    <t>SE-WE-001.005 IPA - Rerate</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.004- Producer Quote - Dental Selection</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.005 - Producer Quote - Under 21 Valid Dental Selection</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.006 Producer Quote - Dental Selection Invalid</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.004.001 Producer Quote - Valid Dental Selection</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.005.001 Producer Quote - Dental Selection Mix</t>
-  </si>
-  <si>
-    <t>SE-MSE-001.003.005.002 Producer Quote - Dental Selection 21 Over</t>
-  </si>
-  <si>
-    <t>SE-MSE-007.002.006 CONFIRM AND ENROLL - MAJOR MED: Enroll Summary Plan</t>
-  </si>
-  <si>
-    <t>SE-MSE-012.001.004 - Cancel Find an Agent Search Page</t>
-  </si>
-  <si>
-    <t>SE-MSE-012.001.004.001.004- Cancel Find an Agent Results Page</t>
-  </si>
-  <si>
-    <t>SE-MSE-0017.002.004 - Native Back Button</t>
-  </si>
-  <si>
-    <t>SE-MSE-021.005.002.002- Other Information: Copy Link - Primary Display</t>
-  </si>
-  <si>
-    <t>SE-MSE-021.005.002.002- Other Information: Copy Link - Spouse And Dependent Display</t>
-  </si>
-  <si>
-    <t>SE-MSE-023.004.005.001 Payment: Billing Address Name - Hyphen</t>
-  </si>
-  <si>
-    <t>SE-MSE-023.004.005.002 Payment: Billing Address Name - Hyphen Clear</t>
-  </si>
-  <si>
-    <t>SE-MSE-033.009.002 Special Enrollment: Applicants Review Page - Full Page Content</t>
-  </si>
-  <si>
-    <t>SE-MSE-033.009.003 - Special Enrollment: Applicants Review Page - Content Box</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002 - Address Verification Service</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.001 - Address Verification Service - Inputs</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.002 - Address Verification Service Inputs: Street Address</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.003 - Address Verification Service - Inputs: City</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.004 - Address Verification Service - Inputs: State</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.005 - Address Verification Service - Inputs: Zip Code</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.006 - Address Verification Service - Outputs</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007 - Address Verification Service - Outputs: Error Content</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.008 - Address Verification Service - Enrollment: Payment Billing Verification</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.009 - Enrollment Payment Address Verification</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.001 - Address Verification Service - Outputs: Error Content</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.002 - Address Verification Service - Outputs: Change Modal Primary Call To Action</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.003 - Address Verification Service - Outputs: Change Modal  Accept</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.004 - Address Verification Service - Outputs: Change Modal  Secondary Call To Action</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.005 - Address Verification Service - Outputs: Change Modal  Reject</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.006 - Address Verification Service - Outputs: Incorrect Modal</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.006.001 - Address Verification Service - Outputs: Incorrect Modal Call to Action</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.006.002 - Address Verification Service - Outputs: Incorrect Modal Close</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.006.003 - Address Verification Service - Outputs: Fatal Error</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.007.006.004 - Address Verification Service - Outputs: Fatal Error Call to Action</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.008.001 - Address Verification Service - Enrollment: Payment Billing Address Verification Error</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.009.001 - Address Verification Service -  Enrollment Payment Residential Address Zip Code Error</t>
-  </si>
-  <si>
-    <t>SE-MSE-035.002.009.002 - Address Verification Service -  Enrollment Payment Residential Address Verification Errors</t>
-  </si>
-  <si>
-    <t>SE-MT-008.001 U65 Eligibility</t>
-  </si>
-  <si>
-    <t>SE-MT-008.002 Med Supp - Display Rates</t>
-  </si>
-  <si>
-    <t>SE-MT-008.003 - OOC</t>
-  </si>
-  <si>
-    <t>SE-MT-008.004 - Application</t>
-  </si>
-  <si>
-    <t>SE-MT-008.005 - Saved Plans</t>
-  </si>
-  <si>
-    <t>SE-MT-008.006 Saved Apps</t>
-  </si>
-  <si>
-    <t>SE-MT-008.002.001 - Price Sort</t>
-  </si>
-  <si>
-    <t>SE-MT-008.002.002 - Default Sort</t>
-  </si>
-  <si>
-    <t>SE-MT-008.002.003 - Content Definitions</t>
-  </si>
-  <si>
-    <t>SE-MT-008.003.001 - OOC Select</t>
-  </si>
-  <si>
-    <t>SE-PM-001.004.008.003  Migration Landing Page - POST PM PUBLIC SITE PAGE: Redirect from RSC Page</t>
-  </si>
-  <si>
-    <t>SE-PM-001.009.001.003 TNB Relationship Code in Multiple Tags</t>
-  </si>
-  <si>
-    <t>SE-PM-001.009.001.003.001 TNB Relationship Code</t>
-  </si>
-  <si>
-    <t>SE-WE-001.004.001 Catastrophic 30</t>
-  </si>
-  <si>
-    <t>SE-WE-001.004.002 Dental 22</t>
-  </si>
-  <si>
-    <t>SE-WE-003.052.000 Ethnicity</t>
-  </si>
-  <si>
-    <t>SE-WE-003.053.000 Communication Preferences</t>
-  </si>
-  <si>
-    <t>SE-WE-003.033.001 Enrollment: Payment -  Address Verification</t>
-  </si>
-  <si>
-    <t>SE-WE-003.033.001.001 Enrollment: Payment -  Residential Address Zip Code Errors</t>
-  </si>
-  <si>
-    <t>SE-WE-003.033.001.002 Enrollment: Payment -  Address Verification Errors</t>
-  </si>
-  <si>
-    <t>SE-WE-003.052.001 Optional</t>
-  </si>
-  <si>
-    <t>SE-WE-003.052 &gt; 1</t>
-  </si>
-  <si>
-    <t>SE-WE-003.053.001 Communication Preferences</t>
-  </si>
-  <si>
-    <t>SE-WE-003.053.002 Communication Preferences_Copy_1</t>
-  </si>
-  <si>
-    <t>SE-WE-006.027.003 Guardian</t>
-  </si>
-  <si>
-    <t>SE-WE-006.027.003.001 Confirm</t>
-  </si>
-  <si>
-    <t>SE-WE-006.027.003.002 Not Confirmed</t>
-  </si>
-  <si>
-    <t>SE-WE-012.006 On Exchange</t>
-  </si>
-  <si>
-    <t>SE-WE-012.007 Special Enroll - Purge Apps</t>
-  </si>
-  <si>
-    <t>SE-WE-012.008 Purge Apps Content</t>
-  </si>
-  <si>
-    <t>SE-WE-012.009 IPA Select</t>
-  </si>
-  <si>
-    <t>SE-WE-014.001 Address Verification Service  - Inputs</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002 Address Verification Service  - Outputs</t>
-  </si>
-  <si>
-    <t>SE-WE-014.001.001 Address Verification Service  - Inputs: Street Address</t>
-  </si>
-  <si>
-    <t>SE-WE-014.001.002 Address Verification Service  - Inputs: City</t>
-  </si>
-  <si>
-    <t>SE-WE-014.001.003 Address Verification Service  - Inputs: State</t>
-  </si>
-  <si>
-    <t>SE-WE-014.001.004 Address Verification Service  - Inputs: Zip Code</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001 Address Verification Service  - Outputs: Errors</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.001 Address Verification Service  - Outputs: Error Content</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.002 Address Verification Service  - Outputs: Change  Modal</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.003 Address Verification Service  - Outputs: Incorrect Modal</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.004 Address Verification Service  - Outputs: Fatal Error</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.002.001 Address Verification Service  - Outputs: Change Modal Primary Call to Action</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.002.002 Address Verification Service  - Outputs: Change Modal Secondary Call to Action</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.002.001.001 Address Verification Service  - Outputs: Change Modal Accept</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.003.001 Address Verification Service  - Outputs: Incorrect Modal Call to Action</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.003.001.001 Address Verification Service  - Outputs: Incorrect Modal Close</t>
-  </si>
-  <si>
-    <t>SE-WE-014.002.001.004.001 Address Verification Service  - Outputs: Fatal Error Call to Actio</t>
-  </si>
-  <si>
-    <t>SE-WE-014.000 - Address Verification Service</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
+  <si>
+    <t xml:space="preserve">SE-065-008.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.004.003.001.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004.001- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004.001.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004.001.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-001.018.004.001.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-005.016.006.004.001.002.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-005.017.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-005.018.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-008.024.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-008.025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.012.017.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-011.001.013.012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.001B.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.003.002.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-013.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.059.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.059.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.062 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.062.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.062.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.063 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.004.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.005.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.005.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.005.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.005.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.064.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.065 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-EI-017.001.066 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-IFA-001.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.004- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.004.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.005.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.005.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-001.003.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-0017.002.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-007.002.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-012.001.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-012.001.004.001.004- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-021.005.002.002- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-023.004.005.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-023.004.005.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-033.009.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-033.009.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.006.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.006.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.006.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.007.006.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.008.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.009.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MSE-035.002.009.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-007.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.002.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.002.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.003.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-MT-008.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-NFR-004.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-O65-008.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-PM-001.004.008.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-PM-001.009.001.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-PM-001.009.001.003.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-PM-007.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-001.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-001.004.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-001.004.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-001.005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.033.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.033.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.033.001.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.052 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.052.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.052.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.053.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.053.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-003.053.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-006.027.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-006.027.003.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-006.027.003.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-012.006 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-012.007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-012.008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-012.009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.001.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.001.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.001.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.002.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.002.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.002.002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.003.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.003.001.001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-WE-014.002.001.004.001 </t>
   </si>
 </sst>
 </file>
@@ -475,10 +466,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,7 +481,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -497,34 +489,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF888888"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF888888"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF888888"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,7 +830,7 @@
   <dimension ref="A1:A147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection sqref="A1:A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -934,672 +905,672 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="2" t="s">
-        <v>146</v>
+      <c r="A147" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>